<commit_message>
Fixed player id assignment
Now correctly accepts input
</commit_message>
<xml_diff>
--- a/Roster Maker Template.xlsx
+++ b/Roster Maker Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\1. Everything Else\Soccer\FIFA\Squad Maker 23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\GitHub\Roster-Maker-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177D995E-4DF9-4904-A8AA-20C719D7CE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A956AD9-FABB-49F8-B326-CBE773ECDCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A600685-B68F-444A-A070-80902014FECE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9A600685-B68F-444A-A070-80902014FECE}"/>
   </bookViews>
   <sheets>
     <sheet name="txt" sheetId="1" r:id="rId1"/>
@@ -420,9 +420,6 @@
     <t>Congo</t>
   </si>
   <si>
-    <t>Côte d'Ivoire</t>
-  </si>
-  <si>
     <t>Djibouti</t>
   </si>
   <si>
@@ -1024,6 +1021,9 @@
   </si>
   <si>
     <t>Less 3k</t>
+  </si>
+  <si>
+    <t>Côte d’Ivoire</t>
   </si>
 </sst>
 </file>
@@ -1395,9 +1395,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1435,7 +1435,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1541,7 +1541,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1683,7 +1683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1693,7 +1693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EE207F-C1F4-4896-9A59-316718883685}">
   <dimension ref="A1:T501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
@@ -1772,32 +1772,32 @@
         <v>40</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G2" s="10">
         <v>90</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N2" s="12">
         <v>16691</v>
@@ -1826,34 +1826,34 @@
         <v>73</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>325</v>
-      </c>
       <c r="D3" s="16" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G3" s="16">
         <v>92</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N3" s="17">
         <v>28021</v>
@@ -12913,7 +12913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A0916C-26DF-4E83-A9FE-06B40F42C2C6}">
   <dimension ref="A1:A224"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13452,532 +13454,532 @@
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>126</v>
+        <v>327</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
@@ -14018,15 +14020,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B2" s="8">
         <v>65</v>
@@ -14034,79 +14036,79 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B12" s="8">
         <v>60</v>
@@ -14114,7 +14116,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B13" s="8">
         <v>61</v>
@@ -14122,15 +14124,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B15" s="8">
         <v>62</v>
@@ -14138,7 +14140,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B16" s="8">
         <v>63</v>
@@ -14146,7 +14148,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B17" s="8">
         <v>64</v>
@@ -14154,7 +14156,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B18" s="8">
         <v>65</v>
@@ -14162,7 +14164,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B19" s="8">
         <v>66</v>
@@ -14170,7 +14172,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B20" s="8">
         <v>67</v>
@@ -14178,7 +14180,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B21" s="8">
         <v>68</v>
@@ -14186,7 +14188,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B22" s="8">
         <v>69</v>
@@ -14194,7 +14196,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B23" s="8">
         <v>70</v>
@@ -14202,7 +14204,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B24" s="8">
         <v>71</v>
@@ -14210,7 +14212,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B25" s="8">
         <v>72</v>
@@ -14218,7 +14220,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B26" s="8">
         <v>73</v>
@@ -14226,7 +14228,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B27" s="8">
         <v>74</v>
@@ -14234,7 +14236,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B28" s="8">
         <v>75</v>
@@ -14242,7 +14244,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B29" s="8">
         <v>76</v>
@@ -14250,7 +14252,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B30" s="8">
         <v>77</v>
@@ -14258,7 +14260,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B31" s="8">
         <v>78</v>
@@ -14266,7 +14268,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B32" s="8">
         <v>79</v>
@@ -14274,7 +14276,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B33" s="8">
         <v>80</v>
@@ -14282,7 +14284,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B34" s="8">
         <v>81</v>
@@ -14290,7 +14292,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B35" s="8">
         <v>82</v>
@@ -14298,7 +14300,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B36" s="8">
         <v>83</v>
@@ -14306,7 +14308,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B37" s="8">
         <v>84</v>
@@ -14314,7 +14316,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B38" s="8">
         <v>85</v>
@@ -14322,7 +14324,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B39" s="8">
         <v>86</v>
@@ -14330,7 +14332,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B40" s="8">
         <v>87</v>
@@ -14338,7 +14340,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B41" s="8">
         <v>88</v>
@@ -14346,10 +14348,10 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -14369,147 +14371,147 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -14529,33 +14531,33 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor update to the template
</commit_message>
<xml_diff>
--- a/Roster Maker Template.xlsx
+++ b/Roster Maker Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\GitHub\Roster-Maker-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A956AD9-FABB-49F8-B326-CBE773ECDCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5891022F-C542-4938-B12F-37D555316765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9A600685-B68F-444A-A070-80902014FECE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A600685-B68F-444A-A070-80902014FECE}"/>
   </bookViews>
   <sheets>
     <sheet name="txt" sheetId="1" r:id="rId1"/>
@@ -1693,7 +1693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EE207F-C1F4-4896-9A59-316718883685}">
   <dimension ref="A1:T501"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
@@ -12913,7 +12913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A0916C-26DF-4E83-A9FE-06B40F42C2C6}">
   <dimension ref="A1:A224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>

</xml_diff>